<commit_message>
Add test cases for screen saver background json interface.
</commit_message>
<xml_diff>
--- a/testdata/testcases.xlsx
+++ b/testdata/testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Function Area</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,19 +50,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SS_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push empty, and pull all screen saver files.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SS_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push all screen saver files, and pull empty.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -87,14 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{
-    "add": [],
-    "delete": [],
-    "update": []
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>POST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,146 +100,189 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.zhengjin.apis.testcases.TestScreenSaverJsonInterface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push all screen saver files, and pull empty.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push empy, and pull all screen saver files.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test11HttpOkWhenPushAllScreenSaverPictures()
+test12PullEmptyWhenPushAllScreenSaverPictures()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
-    "add": [
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 69,
-            "md5": "4e0729ebc2de983f93c3050e54588c26",
-            "mediaId": 301362,
-            "mediaType": 2,
-            "name": "极限挑战 第二季",
-            "size": 3067430,
-            "timestamp": 1466749276000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=4e0729ebc2de983f93c3050e54588c26&amp;w=0&amp;h=0",
-            "weight": 4
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 97,
-            "md5": "d9b59cf8e416ad030aa8c92a88efa376",
-            "mediaId": 302374,
-            "mediaType": 2,
-            "name": "毛泽东三兄弟",
-            "size": 1129173,
-            "timestamp": 1466591829000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=d9b59cf8e416ad030aa8c92a88efa376&amp;w=0&amp;h=0",
-            "weight": 4
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 101,
-            "md5": "645eeada6edd2d4c3ddc2b31a2cdfdf4",
-            "mediaId": 302504,
-            "mediaType": 2,
-            "name": "可爱巧虎岛",
-            "size": 2923118,
-            "timestamp": 1466758848000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=645eeada6edd2d4c3ddc2b31a2cdfdf4&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 99,
-            "md5": "ca7ac4724d87ab1b929188d18db3059f",
-            "mediaId": 0,
-            "mediaType": 0,
-            "name": "日食记",
-            "size": 919433,
-            "timestamp": 1466750751000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=ca7ac4724d87ab1b929188d18db3059f&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 95,
-            "md5": "549539172c654348554210f5d0ab91e7",
-            "mediaId": 302419,
-            "mediaType": 2,
-            "name": "解密",
-            "size": 2945669,
-            "timestamp": 1466497695000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=549539172c654348554210f5d0ab91e7&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 94,
-            "md5": "a7080348dd06753b482642bee36901ef",
-            "mediaId": 302417,
-            "mediaType": 2,
-            "name": "北京遇上西雅图",
-            "size": 3960857,
-            "timestamp": 1466413035000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=a7080348dd06753b482642bee36901ef&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 93,
-            "md5": "feeba34079c2863c1ac834f03033f8d0",
-            "mediaId": 302416,
-            "mediaType": 2,
-            "name": "花样男团",
-            "size": 2745594,
-            "timestamp": 1466396618000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=feeba34079c2863c1ac834f03033f8d0&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 91,
-            "md5": "97fbba63b670b53879e85dbcac2715b3",
-            "mediaId": 0,
-            "mediaType": 0,
-            "name": "加油！美少女",
-            "size": 830922,
-            "timestamp": 1465971022000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=97fbba63b670b53879e85dbcac2715b3&amp;w=0&amp;h=0",
-            "weight": 5
-        },
-        {
-            "begin": 1463390952000,
-            "end": 1469957354000,
-            "id": 89,
-            "md5": "fa7b3835454f286be44abda773879b22",
-            "mediaId": 302211,
-            "mediaType": 2,
-            "name": "梦想合伙人",
-            "size": 2621943,
-            "timestamp": 1465699828000,
-            "type": "内容运营",
-            "url": "http://img.funshion.com/sdw?oid=fa7b3835454f286be44abda773879b22&amp;w=0&amp;h=0",
-            "weight": 5
-        }
-    ],
-    "delete": [],
-    "update": []
+    "retCode": 200,
+    "retMsg": "Success.",
+    "data": {
+        "update": [],
+        "delete": [],
+        "add": [
+            {
+                "mediaId": 301362,
+                "timestamp": 1466749276000,
+                "id": 69,
+                "weight": 4,
+                "name": "极限挑战 第二季",
+                "md5": "4e0729ebc2de983f93c3050e54588c26",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=4e0729ebc2de983f93c3050e54588c26&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 3067430
+            },
+            {
+                "mediaId": 302374,
+                "timestamp": 1466591829000,
+                "id": 97,
+                "weight": 4,
+                "name": "毛泽东三兄弟",
+                "md5": "d9b59cf8e416ad030aa8c92a88efa376",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=d9b59cf8e416ad030aa8c92a88efa376&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 1129173
+            },
+            {
+                "mediaId": 302504,
+                "timestamp": 1466758848000,
+                "id": 101,
+                "weight": 5,
+                "name": "可爱巧虎岛",
+                "md5": "645eeada6edd2d4c3ddc2b31a2cdfdf4",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=645eeada6edd2d4c3ddc2b31a2cdfdf4&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 2923118
+            },
+            {
+                "mediaId": 0,
+                "timestamp": 1466750751000,
+                "id": 99,
+                "weight": 5,
+                "name": "日食记",
+                "md5": "ca7ac4724d87ab1b929188d18db3059f",
+                "type": "内容运营",
+                "mediaType": 0,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=ca7ac4724d87ab1b929188d18db3059f&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 919433
+            },
+            {
+                "mediaId": 302419,
+                "timestamp": 1466497695000,
+                "id": 95,
+                "weight": 5,
+                "name": "解密",
+                "md5": "549539172c654348554210f5d0ab91e7",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=549539172c654348554210f5d0ab91e7&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 2945669
+            },
+            {
+                "mediaId": 302417,
+                "timestamp": 1466413035000,
+                "id": 94,
+                "weight": 5,
+                "name": "北京遇上西雅图",
+                "md5": "a7080348dd06753b482642bee36901ef",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=a7080348dd06753b482642bee36901ef&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 3960857
+            },
+            {
+                "mediaId": 302416,
+                "timestamp": 1466396618000,
+                "id": 93,
+                "weight": 5,
+                "name": "花样男团",
+                "md5": "feeba34079c2863c1ac834f03033f8d0",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=feeba34079c2863c1ac834f03033f8d0&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 2745594
+            },
+            {
+                "mediaId": 0,
+                "timestamp": 1465971022000,
+                "id": 91,
+                "weight": 5,
+                "name": "加油！美少女",
+                "md5": "97fbba63b670b53879e85dbcac2715b3",
+                "type": "内容运营",
+                "mediaType": 0,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=97fbba63b670b53879e85dbcac2715b3&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 830922
+            },
+            {
+                "mediaId": 302211,
+                "timestamp": 1465699828000,
+                "id": 89,
+                "weight": 5,
+                "name": "梦想合伙人",
+                "md5": "fa7b3835454f286be44abda773879b22",
+                "type": "内容运营",
+                "mediaType": 2,
+                "end": 1469957354000,
+                "url": "http://img.funshion.com/sdw?oid=fa7b3835454f286be44abda773879b22&amp;w=0&amp;h=0",
+                "begin": 1463390952000,
+                "size": 2621943
+            }
+        ]
+    }
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.zhengjin.apis.testcases.TestDemo.testReadDataFromExcel</t>
+    <t>{
+    "retCode": 200,
+    "retMsg": "Success.",
+    "data": {
+        "update": [],
+        "delete": [],
+        "add": []
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test21HttpOkWhenPushNoScreenSaverPictures()
+test22PullEmptyForUpdateAndDeleteWhenPushEmpty()
+test23PulledScreenSaverPicturesNameForAddWhenPushEmpty()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -651,9 +674,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -662,17 +685,19 @@
     <col min="1" max="1" width="13.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" style="1" customWidth="1"/>
-    <col min="4" max="5" width="35.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="57.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="60.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="26.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="57.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="60.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24.875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -686,28 +711,31 @@
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -715,32 +743,35 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="162" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -748,30 +779,35 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -782,9 +818,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -795,9 +832,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -808,9 +846,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -821,7 +860,8 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>